<commit_message>
Status Upload - (12-05-2020)
</commit_message>
<xml_diff>
--- a/REVER_DailyTracker_20200505.xlsx
+++ b/REVER_DailyTracker_20200505.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Downloads\DailyTracker-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D714A4-8076-40DD-BAA4-F10EEAA3A1DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BCCC6F-669A-4BDD-9DD8-F4E1A8526E68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{BDBCA639-774E-4870-AA16-72178DF9137C}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="23">
   <si>
     <t>Task</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>Report - Export to Excel</t>
+  </si>
+  <si>
+    <t>Report - Export to PDF</t>
   </si>
 </sst>
 </file>
@@ -1306,7 +1309,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1448,7 +1451,27 @@
       </c>
       <c r="G6" s="21"/>
     </row>
-    <row r="7" spans="1:7" s="4" customFormat="1"/>
+    <row r="7" spans="1:7" s="4" customFormat="1">
+      <c r="A7" s="13">
+        <v>6</v>
+      </c>
+      <c r="B7" s="23">
+        <v>43962</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="24">
+        <v>0.8</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="21"/>
+    </row>
     <row r="8" spans="1:7" s="4" customFormat="1"/>
     <row r="9" spans="1:7" s="4" customFormat="1"/>
     <row r="10" spans="1:7" s="4" customFormat="1"/>

</xml_diff>

<commit_message>
status Update - (12-05-2020)
</commit_message>
<xml_diff>
--- a/REVER_DailyTracker_20200505.xlsx
+++ b/REVER_DailyTracker_20200505.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Downloads\DailyTracker-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BCCC6F-669A-4BDD-9DD8-F4E1A8526E68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3134C0-7108-453A-9A82-50A991C7069A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{BDBCA639-774E-4870-AA16-72178DF9137C}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="24">
   <si>
     <t>Task</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Report - Export to PDF</t>
+  </si>
+  <si>
+    <t>Report - Export to CSV</t>
   </si>
 </sst>
 </file>
@@ -1309,7 +1312,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1472,7 +1475,27 @@
       </c>
       <c r="G7" s="21"/>
     </row>
-    <row r="8" spans="1:7" s="4" customFormat="1"/>
+    <row r="8" spans="1:7" s="4" customFormat="1">
+      <c r="A8" s="13">
+        <v>7</v>
+      </c>
+      <c r="B8" s="23">
+        <v>43963</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="24">
+        <v>0.8</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="21"/>
+    </row>
     <row r="9" spans="1:7" s="4" customFormat="1"/>
     <row r="10" spans="1:7" s="4" customFormat="1"/>
     <row r="11" spans="1:7" s="4" customFormat="1"/>

</xml_diff>

<commit_message>
Status Update - (13-05-2020)
</commit_message>
<xml_diff>
--- a/REVER_DailyTracker_20200505.xlsx
+++ b/REVER_DailyTracker_20200505.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Downloads\DailyTracker-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3134C0-7108-453A-9A82-50A991C7069A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B36D03-3470-4D6D-B8A5-72F2B829599F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{BDBCA639-774E-4870-AA16-72178DF9137C}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="25">
   <si>
     <t>Task</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>Report - Export to CSV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Report </t>
   </si>
 </sst>
 </file>
@@ -1312,7 +1315,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1496,7 +1499,27 @@
       </c>
       <c r="G8" s="21"/>
     </row>
-    <row r="9" spans="1:7" s="4" customFormat="1"/>
+    <row r="9" spans="1:7" s="4" customFormat="1">
+      <c r="A9" s="13">
+        <v>8</v>
+      </c>
+      <c r="B9" s="23">
+        <v>43963</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="24">
+        <v>0.9</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="21"/>
+    </row>
     <row r="10" spans="1:7" s="4" customFormat="1"/>
     <row r="11" spans="1:7" s="4" customFormat="1"/>
     <row r="12" spans="1:7" s="4" customFormat="1"/>

</xml_diff>

<commit_message>
Status Update - (14-05-2020)
</commit_message>
<xml_diff>
--- a/REVER_DailyTracker_20200505.xlsx
+++ b/REVER_DailyTracker_20200505.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Downloads\DailyTracker-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B36D03-3470-4D6D-B8A5-72F2B829599F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C83655D-9C57-4767-9D15-0D066AECCB77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{BDBCA639-774E-4870-AA16-72178DF9137C}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="25">
   <si>
     <t>Task</t>
   </si>
@@ -1315,7 +1315,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1504,7 +1504,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="23">
-        <v>43963</v>
+        <v>43964</v>
       </c>
       <c r="C9" s="21" t="s">
         <v>18</v>
@@ -1520,7 +1520,27 @@
       </c>
       <c r="G9" s="21"/>
     </row>
-    <row r="10" spans="1:7" s="4" customFormat="1"/>
+    <row r="10" spans="1:7" s="4" customFormat="1">
+      <c r="A10" s="13">
+        <v>9</v>
+      </c>
+      <c r="B10" s="23">
+        <v>43965</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="24">
+        <v>1</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="21"/>
+    </row>
     <row r="11" spans="1:7" s="4" customFormat="1"/>
     <row r="12" spans="1:7" s="4" customFormat="1"/>
     <row r="13" spans="1:7" s="4" customFormat="1"/>

</xml_diff>

<commit_message>
Status Update - (15-05-2020)
</commit_message>
<xml_diff>
--- a/REVER_DailyTracker_20200505.xlsx
+++ b/REVER_DailyTracker_20200505.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Downloads\DailyTracker-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C83655D-9C57-4767-9D15-0D066AECCB77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49577934-F206-4B87-B5ED-788BEA32F888}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{BDBCA639-774E-4870-AA16-72178DF9137C}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="26">
   <si>
     <t>Task</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t xml:space="preserve">Report </t>
+  </si>
+  <si>
+    <t>Task - Backend</t>
   </si>
 </sst>
 </file>
@@ -1315,7 +1318,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1541,7 +1544,27 @@
       </c>
       <c r="G10" s="21"/>
     </row>
-    <row r="11" spans="1:7" s="4" customFormat="1"/>
+    <row r="11" spans="1:7" s="4" customFormat="1">
+      <c r="A11" s="13">
+        <v>9</v>
+      </c>
+      <c r="B11" s="23">
+        <v>43966</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="24">
+        <v>1</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="21"/>
+    </row>
     <row r="12" spans="1:7" s="4" customFormat="1"/>
     <row r="13" spans="1:7" s="4" customFormat="1"/>
     <row r="14" spans="1:7" s="4" customFormat="1"/>

</xml_diff>

<commit_message>
Status Update - (18-05-2020)
</commit_message>
<xml_diff>
--- a/REVER_DailyTracker_20200505.xlsx
+++ b/REVER_DailyTracker_20200505.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Downloads\DailyTracker-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49577934-F206-4B87-B5ED-788BEA32F888}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DBF437-5600-4EE9-B22F-2829B7CF1CF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{BDBCA639-774E-4870-AA16-72178DF9137C}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="27">
   <si>
     <t>Task</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>Task - Backend</t>
+  </si>
+  <si>
+    <t>Document &amp; notes Sharing</t>
   </si>
 </sst>
 </file>
@@ -1318,7 +1321,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1546,7 +1549,7 @@
     </row>
     <row r="11" spans="1:7" s="4" customFormat="1">
       <c r="A11" s="13">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="23">
         <v>43966</v>
@@ -1565,7 +1568,27 @@
       </c>
       <c r="G11" s="21"/>
     </row>
-    <row r="12" spans="1:7" s="4" customFormat="1"/>
+    <row r="12" spans="1:7" s="4" customFormat="1">
+      <c r="A12" s="13">
+        <v>11</v>
+      </c>
+      <c r="B12" s="23">
+        <v>43969</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" s="21"/>
+    </row>
     <row r="13" spans="1:7" s="4" customFormat="1"/>
     <row r="14" spans="1:7" s="4" customFormat="1"/>
     <row r="15" spans="1:7" s="4" customFormat="1"/>

</xml_diff>

<commit_message>
Status Update - (19-05-2020)
</commit_message>
<xml_diff>
--- a/REVER_DailyTracker_20200505.xlsx
+++ b/REVER_DailyTracker_20200505.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Downloads\DailyTracker-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DBF437-5600-4EE9-B22F-2829B7CF1CF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6873F6AA-0DE5-43A8-8561-710E0944F563}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{BDBCA639-774E-4870-AA16-72178DF9137C}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="27">
   <si>
     <t>Task</t>
   </si>
@@ -1321,7 +1321,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1589,7 +1589,27 @@
       </c>
       <c r="G12" s="21"/>
     </row>
-    <row r="13" spans="1:7" s="4" customFormat="1"/>
+    <row r="13" spans="1:7" s="4" customFormat="1">
+      <c r="A13" s="13">
+        <v>11</v>
+      </c>
+      <c r="B13" s="23">
+        <v>43970</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="24">
+        <v>0.8</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="21"/>
+    </row>
     <row r="14" spans="1:7" s="4" customFormat="1"/>
     <row r="15" spans="1:7" s="4" customFormat="1"/>
     <row r="16" spans="1:7" s="4" customFormat="1"/>

</xml_diff>

<commit_message>
Status Update - (20-05-2020)
</commit_message>
<xml_diff>
--- a/REVER_DailyTracker_20200505.xlsx
+++ b/REVER_DailyTracker_20200505.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Downloads\DailyTracker-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6873F6AA-0DE5-43A8-8561-710E0944F563}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63FB47D2-EEF2-4B9B-B8BF-D8D43672D7B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{BDBCA639-774E-4870-AA16-72178DF9137C}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="27">
   <si>
     <t>Task</t>
   </si>
@@ -1321,7 +1321,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1591,7 +1591,7 @@
     </row>
     <row r="13" spans="1:7" s="4" customFormat="1">
       <c r="A13" s="13">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="23">
         <v>43970</v>
@@ -1610,7 +1610,27 @@
       </c>
       <c r="G13" s="21"/>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1"/>
+    <row r="14" spans="1:7" s="4" customFormat="1">
+      <c r="A14" s="13">
+        <v>13</v>
+      </c>
+      <c r="B14" s="23">
+        <v>43971</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="24">
+        <v>1</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="21"/>
+    </row>
     <row r="15" spans="1:7" s="4" customFormat="1"/>
     <row r="16" spans="1:7" s="4" customFormat="1"/>
     <row r="17" spans="2:3" s="4" customFormat="1"/>

</xml_diff>

<commit_message>
Status Update - (26-05-2020)
</commit_message>
<xml_diff>
--- a/REVER_DailyTracker_20200505.xlsx
+++ b/REVER_DailyTracker_20200505.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Downloads\DailyTracker-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3338CDD-98D1-480A-A0B1-2C23AF47BACD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{829FAA63-A27D-4FFD-84DA-8C3D9D9761D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{BDBCA639-774E-4870-AA16-72178DF9137C}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="28">
   <si>
     <t>Task</t>
   </si>
@@ -1324,7 +1324,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1676,33 +1676,53 @@
       </c>
       <c r="G16" s="21"/>
     </row>
-    <row r="17" spans="2:3" s="4" customFormat="1"/>
-    <row r="18" spans="2:3" s="4" customFormat="1"/>
-    <row r="19" spans="2:3" s="4" customFormat="1"/>
-    <row r="22" spans="2:3">
+    <row r="17" spans="1:7" s="4" customFormat="1">
+      <c r="A17" s="13">
+        <v>16</v>
+      </c>
+      <c r="B17" s="23">
+        <v>43977</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="24">
+        <v>1</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" s="21"/>
+    </row>
+    <row r="18" spans="1:7" s="4" customFormat="1"/>
+    <row r="19" spans="1:7" s="4" customFormat="1"/>
+    <row r="22" spans="1:7">
       <c r="C22" s="12" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
+    <row r="23" spans="1:7">
       <c r="B23" s="8"/>
       <c r="C23" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="2:3">
+    <row r="24" spans="1:7">
       <c r="B24" s="9"/>
       <c r="C24" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="2:3">
+    <row r="25" spans="1:7">
       <c r="B25" s="10"/>
       <c r="C25" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="2:3">
+    <row r="26" spans="1:7">
       <c r="B26" s="11"/>
       <c r="C26" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Status Update - (27-05-2020)
</commit_message>
<xml_diff>
--- a/REVER_DailyTracker_20200505.xlsx
+++ b/REVER_DailyTracker_20200505.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Downloads\DailyTracker-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{829FAA63-A27D-4FFD-84DA-8C3D9D9761D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17AD2A94-C7DC-4278-8100-C053AAE83839}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{BDBCA639-774E-4870-AA16-72178DF9137C}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="29">
   <si>
     <t>Task</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>RPA-Validations</t>
+  </si>
+  <si>
+    <t>RPA-Sample upload/dowload/email - CSS Design</t>
   </si>
 </sst>
 </file>
@@ -1324,7 +1327,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1697,7 +1700,27 @@
       </c>
       <c r="G17" s="21"/>
     </row>
-    <row r="18" spans="1:7" s="4" customFormat="1"/>
+    <row r="18" spans="1:7" s="4" customFormat="1">
+      <c r="A18" s="13">
+        <v>17</v>
+      </c>
+      <c r="B18" s="23">
+        <v>43978</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="24">
+        <v>0.2</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="21"/>
+    </row>
     <row r="19" spans="1:7" s="4" customFormat="1"/>
     <row r="22" spans="1:7">
       <c r="C22" s="12" t="s">

</xml_diff>